<commit_message>
commiting for flight test
</commit_message>
<xml_diff>
--- a/src/main/java/com/EaseMyTrip/resources/Test Data/FlightSearchInfo.xlsx
+++ b/src/main/java/com/EaseMyTrip/resources/Test Data/FlightSearchInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amit Kumar Das\git\EaseMyTrip\src\main\java\com\EaseMyTrip\resources\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB005EB-68FD-45EB-8194-B6B5A2FBC838}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE75ABFD-4D8D-4CE6-BA3F-0CFFE89E566A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00980611-9D94-4481-BDE2-C19942F6F6F4}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="11">
   <si>
     <t>Departure City</t>
   </si>
@@ -66,9 +66,6 @@
   </si>
   <si>
     <t>Economy</t>
-  </si>
-  <si>
-    <t>Null</t>
   </si>
 </sst>
 </file>
@@ -112,7 +109,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -124,6 +121,17 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,7 +449,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -449,9 +457,9 @@
     <col min="1" max="1" width="11.5546875" customWidth="1"/>
     <col min="2" max="2" width="21.21875" customWidth="1"/>
     <col min="3" max="3" width="24.88671875" customWidth="1"/>
-    <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="22.44140625" customWidth="1"/>
+    <col min="4" max="4" width="21" style="7" customWidth="1"/>
+    <col min="5" max="5" width="20" style="7" customWidth="1"/>
+    <col min="6" max="6" width="22.44140625" style="9" customWidth="1"/>
     <col min="7" max="7" width="20.44140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -465,13 +473,13 @@
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="8" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -491,10 +499,10 @@
       <c r="D2" s="4">
         <v>44075</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="3">
+      <c r="E2" s="4">
+        <v>44075</v>
+      </c>
+      <c r="F2" s="5">
         <v>1</v>
       </c>
       <c r="G2" s="3" t="s">
@@ -514,10 +522,10 @@
       <c r="D3" s="4">
         <v>44076</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="3">
+      <c r="E3" s="4">
+        <v>44076</v>
+      </c>
+      <c r="F3" s="5">
         <v>1</v>
       </c>
       <c r="G3" s="3" t="s">
@@ -537,10 +545,10 @@
       <c r="D4" s="4">
         <v>44077</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="3">
+      <c r="E4" s="4">
+        <v>44077</v>
+      </c>
+      <c r="F4" s="5">
         <v>1</v>
       </c>
       <c r="G4" s="3" t="s">
@@ -560,10 +568,10 @@
       <c r="D5" s="4">
         <v>44078</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="3">
+      <c r="E5" s="4">
+        <v>44078</v>
+      </c>
+      <c r="F5" s="5">
         <v>1</v>
       </c>
       <c r="G5" s="3" t="s">
@@ -583,10 +591,10 @@
       <c r="D6" s="4">
         <v>44079</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="3">
+      <c r="E6" s="4">
+        <v>44079</v>
+      </c>
+      <c r="F6" s="5">
         <v>1</v>
       </c>
       <c r="G6" s="3" t="s">
@@ -606,10 +614,10 @@
       <c r="D7" s="4">
         <v>44080</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="3">
+      <c r="E7" s="4">
+        <v>44080</v>
+      </c>
+      <c r="F7" s="5">
         <v>1</v>
       </c>
       <c r="G7" s="3" t="s">
@@ -629,10 +637,10 @@
       <c r="D8" s="4">
         <v>44081</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="3">
+      <c r="E8" s="4">
+        <v>44081</v>
+      </c>
+      <c r="F8" s="5">
         <v>1</v>
       </c>
       <c r="G8" s="3" t="s">

</xml_diff>

<commit_message>
fixed stale element reference exception
</commit_message>
<xml_diff>
--- a/src/main/java/com/EaseMyTrip/resources/Test Data/FlightSearchInfo.xlsx
+++ b/src/main/java/com/EaseMyTrip/resources/Test Data/FlightSearchInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amit Kumar Das\git\EaseMyTrip\src\main\java\com\EaseMyTrip\resources\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62204774-360F-4EA8-8DCD-012C86D1CB9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3979E053-6D85-47B4-B3E3-8BB2B679C5DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00980611-9D94-4481-BDE2-C19942F6F6F4}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="16">
   <si>
     <t>Departure City</t>
   </si>
@@ -66,6 +66,21 @@
   </si>
   <si>
     <t>Economy</t>
+  </si>
+  <si>
+    <t>Delhi</t>
+  </si>
+  <si>
+    <t>Hyderabad</t>
+  </si>
+  <si>
+    <t>Ahmedabad</t>
+  </si>
+  <si>
+    <t>Kota</t>
+  </si>
+  <si>
+    <t>Bangalore</t>
   </si>
 </sst>
 </file>
@@ -109,7 +124,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -132,6 +147,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F65C4A6-3D23-42D4-A9AF-9E9E905661E0}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -497,10 +515,10 @@
         <v>8</v>
       </c>
       <c r="D2" s="4">
-        <v>44079</v>
+        <v>44110</v>
       </c>
       <c r="E2" s="4">
-        <v>44079</v>
+        <v>44110</v>
       </c>
       <c r="F2" s="8">
         <v>1</v>
@@ -514,16 +532,16 @@
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="D3" s="4">
-        <v>44080</v>
+        <v>44110</v>
       </c>
       <c r="E3" s="4">
-        <v>44080</v>
+        <v>44110</v>
       </c>
       <c r="F3" s="8">
         <v>1</v>
@@ -537,21 +555,113 @@
         <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="4">
+        <v>44142</v>
+      </c>
+      <c r="E4" s="4">
+        <v>44142</v>
+      </c>
+      <c r="F4" s="8">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="4">
-        <v>44081</v>
-      </c>
-      <c r="E4" s="4">
-        <v>44081</v>
-      </c>
-      <c r="F4" s="8">
-        <v>1</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="D5" s="10">
+        <v>44173</v>
+      </c>
+      <c r="E5" s="10">
+        <v>44173</v>
+      </c>
+      <c r="F5" s="8">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="10">
+        <v>44216</v>
+      </c>
+      <c r="E6" s="10">
+        <v>44216</v>
+      </c>
+      <c r="F6" s="8">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="10">
+        <v>44247</v>
+      </c>
+      <c r="E7" s="10">
+        <v>44247</v>
+      </c>
+      <c r="F7" s="8">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="10">
+        <v>44275</v>
+      </c>
+      <c r="E8" s="10">
+        <v>44275</v>
+      </c>
+      <c r="F8" s="8">
+        <v>1</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Committing for filter verification changes, data provider class, flight search list excel changes and code refactoring for flight test class
</commit_message>
<xml_diff>
--- a/src/main/java/com/EaseMyTrip/resources/Test Data/FlightSearchInfo.xlsx
+++ b/src/main/java/com/EaseMyTrip/resources/Test Data/FlightSearchInfo.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amit Kumar Das\git\EaseMyTrip\src\main\java\com\EaseMyTrip\resources\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3979E053-6D85-47B4-B3E3-8BB2B679C5DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21AE75F4-8561-41A2-A1E9-D07C6F77E25B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00980611-9D94-4481-BDE2-C19942F6F6F4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00980611-9D94-4481-BDE2-C19942F6F6F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="16">
   <si>
     <t>Departure City</t>
   </si>
@@ -466,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F65C4A6-3D23-42D4-A9AF-9E9E905661E0}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -669,4 +670,74 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2429F156-D4A0-440A-9A4F-3578288BFA2D}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="17.77734375" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="5" max="5" width="23.21875" customWidth="1"/>
+    <col min="6" max="6" width="23.6640625" customWidth="1"/>
+    <col min="7" max="7" width="25.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="4">
+        <v>44110</v>
+      </c>
+      <c r="E2" s="4">
+        <v>44110</v>
+      </c>
+      <c r="F2" s="8">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>